<commit_message>
att dados ana pascoini
</commit_message>
<xml_diff>
--- a/data-raw/ana-paschoini/da_ana_paschoini.xlsx
+++ b/data-raw/ana-paschoini/da_ana_paschoini.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:D212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -380,6 +380,11 @@
           <t>origem</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>upi_vendeu</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -395,6 +400,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -410,6 +420,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -425,6 +440,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -440,6 +460,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -455,6 +480,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -470,6 +500,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -485,6 +520,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -500,6 +540,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -515,6 +560,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -530,6 +580,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -545,6 +600,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -560,6 +620,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -575,6 +640,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -590,6 +660,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -605,6 +680,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -620,6 +700,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -635,6 +720,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -650,6 +740,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -665,6 +760,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -680,6 +780,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -695,6 +800,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -710,6 +820,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -725,6 +840,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -740,6 +860,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -755,6 +880,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -770,6 +900,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -785,6 +920,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -800,6 +940,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -815,6 +960,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -830,6 +980,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -845,6 +1000,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -860,6 +1020,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -875,6 +1040,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -890,6 +1060,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -905,6 +1080,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -920,6 +1100,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -935,6 +1120,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -950,6 +1140,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -965,6 +1160,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -980,6 +1180,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -995,6 +1200,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1010,6 +1220,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1025,6 +1240,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1040,6 +1260,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1055,6 +1280,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1070,6 +1300,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1085,6 +1320,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1100,6 +1340,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1115,6 +1360,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1130,6 +1380,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1145,6 +1400,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1160,6 +1420,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1175,6 +1440,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1190,6 +1460,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1205,6 +1480,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1220,6 +1500,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1235,6 +1520,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1250,6 +1540,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1265,6 +1560,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1280,6 +1580,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1295,6 +1600,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1310,6 +1620,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1325,6 +1640,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1340,6 +1660,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1355,6 +1680,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1370,6 +1700,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1385,6 +1720,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1400,6 +1740,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1415,6 +1760,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1430,6 +1780,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1445,6 +1800,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1460,6 +1820,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1475,6 +1840,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1490,6 +1860,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1505,6 +1880,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1520,6 +1900,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1535,6 +1920,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1550,6 +1940,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1565,6 +1960,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1580,6 +1980,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1595,6 +2000,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1610,6 +2020,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1625,6 +2040,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1640,6 +2060,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1655,6 +2080,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1670,6 +2100,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1685,6 +2120,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1700,6 +2140,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1715,6 +2160,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1730,6 +2180,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1745,6 +2200,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1760,6 +2220,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1775,6 +2240,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1790,6 +2260,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1805,6 +2280,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1820,6 +2300,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1835,6 +2320,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1850,6 +2340,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1865,6 +2360,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1880,6 +2380,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1895,6 +2400,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1910,6 +2420,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -1925,6 +2440,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -1940,6 +2460,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -1955,6 +2480,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1970,6 +2500,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -1985,6 +2520,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2000,6 +2540,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2015,6 +2560,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2030,6 +2580,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2045,6 +2600,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2060,6 +2620,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2075,6 +2640,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2090,6 +2660,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2105,6 +2680,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2120,6 +2700,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2135,6 +2720,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2150,6 +2740,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2165,6 +2760,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2180,6 +2780,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2195,6 +2800,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2210,6 +2820,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2223,6 +2838,11 @@
       <c r="C124" t="inlineStr">
         <is>
           <t>SP</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Não</t>
         </is>
       </c>
     </row>

</xml_diff>